<commit_message>
updates variable name harmonization with label types
</commit_message>
<xml_diff>
--- a/data-raw/var_lab_dict.xlsx
+++ b/data-raw/var_lab_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\eurobarometer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29562BC-AA23-4A52-A646-A98100832D39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938BB6EB-1E8A-44EC-9D9E-D9701A3B03FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{255F3ACE-66B4-45EB-8605-23D9930ED332}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="333">
   <si>
     <t>^cap_</t>
   </si>
@@ -1008,6 +1008,27 @@
   </si>
   <si>
     <t>^sex$</t>
+  </si>
+  <si>
+    <t>justice$</t>
+  </si>
+  <si>
+    <t>court-of-justice</t>
+  </si>
+  <si>
+    <t>court_of_justice</t>
+  </si>
+  <si>
+    <t>eu_court_of_justice</t>
+  </si>
+  <si>
+    <t>rely_on</t>
+  </si>
+  <si>
+    <t>prbl</t>
+  </si>
+  <si>
+    <t>problem</t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE4E4BF-B04C-467E-B8C0-FD4C5C180FD6}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1762,882 +1783,907 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>332</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>331</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>285</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>286</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>285</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>31</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C52" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>36</v>
+        <v>210</v>
+      </c>
+      <c r="C53" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>324</v>
+        <v>128</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>129</v>
+        <v>324</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>38</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>212</v>
+        <v>38</v>
       </c>
       <c r="C57" t="s">
-        <v>213</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+      <c r="D58" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C59" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
-      </c>
-      <c r="D60" t="s">
-        <v>220</v>
-      </c>
-      <c r="E60" t="s">
-        <v>221</v>
-      </c>
-      <c r="F60" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>39</v>
+        <v>218</v>
+      </c>
+      <c r="C61" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" t="s">
+        <v>220</v>
+      </c>
+      <c r="E61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F61" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C65" t="s">
-        <v>224</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C66" t="s">
-        <v>226</v>
-      </c>
-      <c r="D66" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>43</v>
+        <v>225</v>
+      </c>
+      <c r="C67" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>322</v>
+        <v>143</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>323</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>322</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C72" t="s">
-        <v>229</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>47</v>
+        <v>228</v>
+      </c>
+      <c r="C73" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>289</v>
+        <v>146</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>290</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>49</v>
+        <v>290</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>288</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>287</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C78" t="s">
-        <v>231</v>
+        <v>288</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>293</v>
+        <v>147</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>294</v>
+        <v>230</v>
+      </c>
+      <c r="C79" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>291</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>317</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>316</v>
+        <v>149</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C83" t="s">
-        <v>233</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>316</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>51</v>
+        <v>232</v>
+      </c>
+      <c r="C84" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>306</v>
+        <v>151</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>307</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>306</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>53</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C91" t="s">
-        <v>235</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>57</v>
+        <v>234</v>
+      </c>
+      <c r="C92" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>157</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>301</v>
+        <v>57</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>300</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>58</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>160</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>161</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>162</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>163</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>164</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>165</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>302</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>304</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>166</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>167</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>168</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>327</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>170</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>171</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C111" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>172</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>173</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C111" t="s">
-        <v>241</v>
-      </c>
-      <c r="D111" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>174</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C112" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>71</v>
+        <v>240</v>
+      </c>
+      <c r="C113" t="s">
+        <v>241</v>
+      </c>
+      <c r="D113" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>271</v>
+        <v>72</v>
       </c>
       <c r="C114" t="s">
-        <v>270</v>
-      </c>
-      <c r="D114" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>269</v>
+        <v>175</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C115" t="s">
-        <v>264</v>
-      </c>
-      <c r="D115" t="s">
-        <v>265</v>
-      </c>
-      <c r="E115" t="s">
-        <v>276</v>
-      </c>
-      <c r="F115" t="s">
-        <v>278</v>
+        <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>72</v>
+        <v>271</v>
+      </c>
+      <c r="C116" t="s">
+        <v>270</v>
+      </c>
+      <c r="D116" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>269</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="C117" t="s">
-        <v>245</v>
+        <v>264</v>
+      </c>
+      <c r="D117" t="s">
+        <v>265</v>
+      </c>
+      <c r="E117" t="s">
+        <v>276</v>
+      </c>
+      <c r="F117" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>318</v>
+        <v>174</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>319</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>320</v>
+        <v>177</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>321</v>
+        <v>244</v>
+      </c>
+      <c r="C119" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>178</v>
+        <v>320</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C121" t="s">
-        <v>247</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C122" t="s">
-        <v>249</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C123" t="s">
-        <v>251</v>
-      </c>
-      <c r="D123" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C124" t="s">
-        <v>254</v>
+        <v>249</v>
+      </c>
+      <c r="D124" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>73</v>
+        <v>250</v>
+      </c>
+      <c r="C125" t="s">
+        <v>251</v>
+      </c>
+      <c r="D125" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>74</v>
+        <v>253</v>
+      </c>
+      <c r="C126" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C130" t="s">
-        <v>272</v>
+        <v>76</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>273</v>
+        <v>186</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C131" t="s">
-        <v>275</v>
+        <v>77</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>78</v>
+        <v>255</v>
+      </c>
+      <c r="C132" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>79</v>
+        <v>274</v>
+      </c>
+      <c r="C133" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>296</v>
+        <v>188</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>297</v>
+        <v>78</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>298</v>
+        <v>189</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>299</v>
+        <v>79</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>190</v>
+        <v>298</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C137" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>191</v>
+        <v>308</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>80</v>
+        <v>309</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>81</v>
+        <v>256</v>
+      </c>
+      <c r="C139" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>191</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>192</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>193</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>